<commit_message>
resolving binary shapes, in v1.x
</commit_message>
<xml_diff>
--- a/shapes.xlsx
+++ b/shapes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/waok2hurricane/Desktop/lazima/projects/play-area/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8DC7F1-0AF2-D54E-A1A0-A91CDE1E73B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3650B9FE-9C99-9243-A163-39BD247D87B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{33E7EB2D-2B52-BB4B-A71E-BD1F0E428788}"/>
   </bookViews>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">square </t>
   </si>
   <si>
-    <t>circle</t>
+    <t>rectangle</t>
   </si>
 </sst>
 </file>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D2C004-123D-A14C-B3B9-505451C22602}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -408,8 +408,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>